<commit_message>
Proyecto Final Lattenero Terminado
</commit_message>
<xml_diff>
--- a/Casos_de_prueba_Leonardo_Lattenero.xlsx
+++ b/Casos_de_prueba_Leonardo_Lattenero.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo\Desktop\VISUAL STUDIO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo\ProyectoFinalLattenero\ProyectoFinalLatt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64D81C8-814E-4751-B783-3B2F97AA8672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1880800B-6F40-4B4F-8F0E-C24C0242C6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0B22D43C-FFEB-47A7-9EB6-212410DAF462}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -96,49 +95,108 @@
     <t>Agregar Avatar</t>
   </si>
   <si>
-    <t>la URL agregarAvatar deja agregar un Avatar a eleccion del usuario en la carpeta media.</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
-    <t>Permite que los usuarios se logueen con su "username" y "password"</t>
-  </si>
-  <si>
     <t>Resultados Reales</t>
   </si>
   <si>
-    <t>A traves de la URL agregarAvatar, permitir agregar una foto de usuario</t>
-  </si>
-  <si>
-    <t>Debe permitirque los usuarios se logueen con su nombre de ususario y contraseña</t>
-  </si>
-  <si>
     <t>Debe llevar al inicio del Blog</t>
   </si>
   <si>
     <t>Lleva al inicio del blog</t>
   </si>
   <si>
-    <t>Debe llevar a una pagina que cuente sobre el autor del blog</t>
-  </si>
-  <si>
     <t>Lleva a una pagina que hace una breve descripcion del autor del Fitness Blog</t>
   </si>
   <si>
-    <t>Click en boton Logout</t>
-  </si>
-  <si>
     <t>Debe desloguear al usuario y mostrar menos opciones en el NavBar</t>
   </si>
   <si>
-    <t>Deslogua al usuario y solo permite ir a inicio (home), registrar usuario y "about"</t>
-  </si>
-  <si>
-    <t>Click en home del NavBar</t>
-  </si>
-  <si>
-    <t>Click en about del NavBar</t>
+    <t>Debe permitir que los usuarios se logueen con su nombre de ususario y contraseña</t>
+  </si>
+  <si>
+    <t>Permite que los usuarios se logueen con su "username" y "password" a traves del boton Login.</t>
+  </si>
+  <si>
+    <t>Deslogua al usuario y solo permite ir a inicio (home), registrar usuario y "about" y boton Login</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click en </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>home</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> del NavBar</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click en </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>about</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> del NavBar</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click en boton </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Logout</t>
+    </r>
+  </si>
+  <si>
+    <t>A traves de la URL /accounts/login/agregarAvatar/, permitir agregar una foto de usuario</t>
+  </si>
+  <si>
+    <t>la URL /accounts/login/agregarAvatar/ deja agregar un Avatar a eleccion del usuario en la carpeta avatares.</t>
+  </si>
+  <si>
+    <t>Debe llevar a una pagina que cuente sobre el autor del blog a traves de la ruta /accounts/login/about/</t>
   </si>
 </sst>
 </file>
@@ -488,35 +546,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -536,43 +595,29 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -580,17 +625,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -598,32 +667,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -631,11 +685,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -953,493 +1013,427 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E4BB0E-2660-40A4-9E48-96551EC18EE5}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.81640625" customWidth="1"/>
-    <col min="8" max="8" width="13.453125" customWidth="1"/>
+    <col min="6" max="6" width="27.6328125" customWidth="1"/>
+    <col min="8" max="8" width="17.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="18"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="18"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="21"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="17"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="18"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55" t="s">
+      <c r="C10" s="23"/>
+      <c r="D10" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="55"/>
-      <c r="F10" s="54" t="s">
+      <c r="E10" s="23"/>
+      <c r="F10" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G10" s="55" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55" t="s">
+      <c r="G10" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="55"/>
+      <c r="J10" s="23"/>
     </row>
     <row r="11" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>1</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="24">
         <v>44958</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="13" t="s">
+      <c r="C11" s="25"/>
+      <c r="D11" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="8"/>
+      <c r="E11" s="25"/>
       <c r="F11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="7" t="s">
+      <c r="H11" s="43"/>
+      <c r="I11" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="J11" s="8"/>
-    </row>
-    <row r="12" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="J11" s="25"/>
+    </row>
+    <row r="12" spans="1:10" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>2</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="24">
         <v>44958</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="5" t="s">
+      <c r="C12" s="25"/>
+      <c r="D12" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="6"/>
+      <c r="E12" s="54"/>
       <c r="F12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="10"/>
-      <c r="I12" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="36"/>
+      <c r="I12" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="J12" s="8"/>
+      <c r="J12" s="25"/>
     </row>
     <row r="13" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>3</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="24">
         <v>44958</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="10"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="36"/>
       <c r="F13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="42"/>
-      <c r="I13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="45"/>
+      <c r="I13" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="J13" s="8"/>
-    </row>
-    <row r="14" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="J13" s="25"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>4</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="24">
         <v>44958</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="10"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="36"/>
       <c r="F14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="10"/>
-      <c r="I14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="36"/>
+      <c r="I14" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="J14" s="8"/>
-    </row>
-    <row r="15" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="43">
+      <c r="J14" s="25"/>
+    </row>
+    <row r="15" spans="1:10" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="11">
         <v>5</v>
       </c>
-      <c r="B15" s="35">
+      <c r="B15" s="30">
         <v>44958</v>
       </c>
-      <c r="C15" s="36"/>
+      <c r="C15" s="31"/>
       <c r="D15" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="38"/>
+      <c r="F15" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="38"/>
-      <c r="F15" s="39" t="s">
+      <c r="G15" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="38"/>
+      <c r="I15" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" s="31"/>
+    </row>
+    <row r="16" spans="1:10" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="12">
+        <v>6</v>
+      </c>
+      <c r="B16" s="32">
+        <v>44958</v>
+      </c>
+      <c r="C16" s="33"/>
+      <c r="D16" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="40"/>
+      <c r="F16" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="H15" s="38"/>
-      <c r="I15" s="40" t="s">
+      <c r="H16" s="40"/>
+      <c r="I16" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="J15" s="36"/>
-    </row>
-    <row r="16" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="46">
-        <v>6</v>
-      </c>
-      <c r="B16" s="47">
-        <v>44958</v>
-      </c>
-      <c r="C16" s="48"/>
-      <c r="D16" s="49" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="50"/>
-      <c r="F16" s="51" t="s">
-        <v>31</v>
-      </c>
-      <c r="G16" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="H16" s="50"/>
-      <c r="I16" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="J16" s="53"/>
+      <c r="J16" s="51"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="31"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="32"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="25"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="27"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="25"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="27"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="29"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="25"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="27"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="29"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="25"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="27"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="29"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="31"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="32"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="31"/>
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="31"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A25" s="31"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
+      <c r="A25" s="8"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" s="31"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
+      <c r="A26" s="8"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" s="31"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="32"/>
-      <c r="J27" s="32"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="84">
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="I18:J18"/>
@@ -1456,11 +1450,74 @@
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D13:E13"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
     <mergeCell ref="I23:J23"/>
     <mergeCell ref="I24:J24"/>
     <mergeCell ref="I25:J25"/>
     <mergeCell ref="I26:J26"/>
     <mergeCell ref="I27:J27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="G8:J8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>